<commit_message>
rafaels diary update 2020-02-23
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7C1A60-58EF-47D4-9300-801C0B87913D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689D4776-FBAB-437D-AF78-9EA8E6381A97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -277,6 +277,48 @@
   </si>
   <si>
     <t>Decided when we should meet and what we should do those days</t>
+  </si>
+  <si>
+    <t>2:30PM - 5:00 PM</t>
+  </si>
+  <si>
+    <t>Finish and resubmit assignment 2</t>
+  </si>
+  <si>
+    <t>We rewrote the document using higher level abstractions and went our discovery process more throughly</t>
+  </si>
+  <si>
+    <t>Structuring the document into paragraphs and making links to our diagrams makes our document more understandable</t>
+  </si>
+  <si>
+    <t>2:00PM - 7:10 PM</t>
+  </si>
+  <si>
+    <t>Exhausted</t>
+  </si>
+  <si>
+    <t>Explained the social context, identified interesting pull requests and issues, and explained the architecture of our project in a concise document</t>
+  </si>
+  <si>
+    <t>Finish and deliver our project assignment #4</t>
+  </si>
+  <si>
+    <t>Since we had already worked on the essential features, we already had a general understanding of our project, so it was easier to understand the architecture because we knew the exact routes we had to study</t>
+  </si>
+  <si>
+    <t>5:00PM - 7:00 PM</t>
+  </si>
+  <si>
+    <t>Learn new expert key practices, what is social context, and how does architecture can help understanding code</t>
+  </si>
+  <si>
+    <t>Understood what social context is and how it might affect our decisions when choosing a project, and  how professionals use architecture as a comprehension tool</t>
+  </si>
+  <si>
+    <t>Feeling ok</t>
+  </si>
+  <si>
+    <t>It was good to hear our guest speakers give suggestions on how to introduce new members to the project and team, and how they guide them in the proper way to contribute</t>
   </si>
 </sst>
 </file>
@@ -459,11 +501,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -785,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,24 +837,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1215,42 +1257,84 @@
       <c r="D23" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>75</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+    <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>43880</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>43881</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>43882</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>

</xml_diff>